<commit_message>
Rename RolHorizon as Horizon
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_ed.xlsx
+++ b/ams/cases/ieee14/ieee14_ed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1635005D-3976-AD4A-83D2-74D031AD7D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B77313-6085-3040-977F-23B83D04C59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Area" sheetId="7" r:id="rId8"/>
     <sheet name="GCost" sheetId="8" r:id="rId9"/>
     <sheet name="Region" sheetId="10" r:id="rId10"/>
-    <sheet name="RolHorizon" sheetId="13" r:id="rId11"/>
+    <sheet name="Horizon" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1369,7 +1369,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[WIP] ED, fix constr rampu and rampd
</commit_message>
<xml_diff>
--- a/ams/cases/ieee14/ieee14_ed.xlsx
+++ b/ams/cases/ieee14/ieee14_ed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BC1038-3659-634E-BD98-9A46E4591408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA9A288-102D-E249-9F26-357CA046BF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36480" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="263">
   <si>
     <t>uid</t>
   </si>
@@ -816,18 +816,28 @@
   </si>
   <si>
     <t>scale</t>
+  </si>
+  <si>
+    <t>R30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -920,22 +930,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1386,7 +1402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD46B62-3884-454B-83D5-13A7DC1C4BB6}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1470,7 +1486,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2156,13 +2172,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="20" max="20" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2220,8 +2241,11 @@
       <c r="S1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2276,8 +2300,11 @@
       <c r="S2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2332,8 +2359,11 @@
       <c r="S3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2388,8 +2418,11 @@
       <c r="S4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2443,6 +2476,9 @@
       </c>
       <c r="S5" t="s">
         <v>103</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2455,13 +2491,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="21" max="21" width="11" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2522,8 +2563,11 @@
       <c r="T1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2580,6 +2624,9 @@
       </c>
       <c r="T2" t="s">
         <v>14</v>
+      </c>
+      <c r="U2" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>